<commit_message>
Correzinoe nome foglio di lavoro, in TestCases
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
+++ b/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://werfen-my.sharepoint.com/personal/mepure_werfen_com/Documents/Documenti/PNRR/NEW_TEST_CASE/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3E15204-9648-4B0A-BE41-C6E46B6496F8}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22DFD6B7-6F8A-43B1-A21E-6D782B2819B2}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{45719620-2FD1-4552-A135-64BB57A71FCF}"/>
+    <workbookView xWindow="2557" yWindow="3382" windowWidth="17176" windowHeight="10343" xr2:uid="{45719620-2FD1-4552-A135-64BB57A71FCF}"/>
   </bookViews>
   <sheets>
-    <sheet name="TEST_CASE" sheetId="2" r:id="rId1"/>
+    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -827,6 +827,20 @@
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
       <protection locked="0"/>
@@ -845,34 +859,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -890,10 +890,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1196,7 +1192,7 @@
   <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1246,14 +1242,14 @@
       <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.45">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="20"/>
+      <c r="D2" s="24"/>
       <c r="E2" s="14"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
@@ -1272,14 +1268,14 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="20"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="14"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -1298,13 +1294,13 @@
       <c r="T3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="24" t="s">
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="27"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="19"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
@@ -1322,12 +1318,12 @@
       <c r="T4" s="16"/>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="24" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="14"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -1346,9 +1342,9 @@
       <c r="T5" s="16"/>
     </row>
     <row r="6" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="15"/>

</xml_diff>

<commit_message>
Correzione file per pdf errato
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
+++ b/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://werfen-my.sharepoint.com/personal/mepure_werfen_com/Documents/Documenti/PNRR/NEW_TEST_CASE/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35DA487D-181C-488D-8E5B-C2CCAEC25A42}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A52B60-BA45-4C52-AA31-6AA333CAF06F}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45719620-2FD1-4552-A135-64BB57A71FCF}"/>
   </bookViews>
@@ -416,51 +416,6 @@
     <t>Il campo in esame è sempre presente</t>
   </si>
   <si>
-    <t>2023-04-03T18:33:43Z</t>
-  </si>
-  <si>
-    <t>806b20187421400e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4ed3c6c2dd078a9c27c0565da3a3453ae86ca8178f55696f6b2357ca63efd678.ff3bbc12ef^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T18:35:19Z</t>
-  </si>
-  <si>
-    <t>e8ab3fa92fad0b9b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4ed3c6c2dd078a9c27c0565da3a3453ae86ca8178f55696f6b2357ca63efd678.2c37635a89^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T18:35:54Z</t>
-  </si>
-  <si>
-    <t>72800b76c4c18459</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4ed3c6c2dd078a9c27c0565da3a3453ae86ca8178f55696f6b2357ca63efd678.068efe7d27^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T18:36:59Z</t>
-  </si>
-  <si>
-    <t>c230ae16c6c950fc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4ed3c6c2dd078a9c27c0565da3a3453ae86ca8178f55696f6b2357ca63efd678.46888fd5a5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-03T18:37:33Z</t>
-  </si>
-  <si>
-    <t>e7dcc9f24feff244</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.4ed3c6c2dd078a9c27c0565da3a3453ae86ca8178f55696f6b2357ca63efd678.40ee9c6dbb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-04-03T19:17:59Z</t>
   </si>
   <si>
@@ -471,6 +426,51 @@
   </si>
   <si>
     <t>Jwt sempre valorizzato con i valori richiesti</t>
+  </si>
+  <si>
+    <t>2023-04-04T08:08:12Z</t>
+  </si>
+  <si>
+    <t>10c0f47781b3d506</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.fb45f3577b696e54209bc2b936b93d8a70a7fa3458a50e694282b1d5799afd9f.d1e963401f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T08:10:56Z</t>
+  </si>
+  <si>
+    <t>889bd3999b120994</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.64f74863595b6c2e7c8715ebaf432ceabb5091659c9369541a2641e60a80aeb3.4e77841d9f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T08:13:05Z</t>
+  </si>
+  <si>
+    <t>1805a5034fd5b06d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.2d257b5b8c756775146115c50b0d97851c0a657dfb3d22fe8561cfe9c1f1e2b4.babb7c65c2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-04T08:18:58Z</t>
+  </si>
+  <si>
+    <t>9d2a04ab2ca6ec02</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.b3f88f87fbd4d91f876411f8dd396e4d8491a8506178c07d2b78c911a0f8b320.94f09de098^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>07ec4b2c686c1c09</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.30.2b51ae544a471226d473780a5f9f0ac3714f12b3c9f8a93d4efe1d102774d3b3.362a84b5eb^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>22023-04-04T08:21:07Z</t>
   </si>
 </sst>
 </file>
@@ -872,6 +872,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1173,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762FDFC5-2362-40DA-8182-D4388668A5DB}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1424,16 +1428,16 @@
         <v>18</v>
       </c>
       <c r="F8" s="8">
-        <v>45019</v>
+        <v>45020</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>19</v>
@@ -1476,16 +1480,16 @@
         <v>21</v>
       </c>
       <c r="F9" s="8">
-        <v>45019</v>
+        <v>45020</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>19</v>
@@ -1528,16 +1532,16 @@
         <v>23</v>
       </c>
       <c r="F10" s="8">
-        <v>45019</v>
+        <v>45020</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>19</v>
@@ -1580,16 +1584,16 @@
         <v>25</v>
       </c>
       <c r="F11" s="8">
-        <v>45019</v>
+        <v>45020</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>19</v>
@@ -1632,16 +1636,16 @@
         <v>27</v>
       </c>
       <c r="F12" s="8">
-        <v>45019</v>
+        <v>45020</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>19</v>
@@ -1729,7 +1733,7 @@
         <v>29</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -1839,13 +1843,13 @@
         <v>45019</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Aggiornamento gestione test K
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
+++ b/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://werfen-my.sharepoint.com/personal/mepure_werfen_com/Documents/Documenti/PNRR/NEW_TEST_CASE/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76A52B60-BA45-4C52-AA31-6AA333CAF06F}"/>
+  <xr:revisionPtr revIDLastSave="197" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8D1B0AD-F5ED-4AF2-9019-9DCBD76A9A03}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45719620-2FD1-4552-A135-64BB57A71FCF}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15120" xr2:uid="{45719620-2FD1-4552-A135-64BB57A71FCF}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="2" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -316,10 +316,6 @@
       <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" con un token jwt non valido a causa della mancanza di uno o più campi obbligatori al fine di testare la gestione dell'errore sul token (status code 403), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.</t>
     </r>
-  </si>
-  <si>
-    <t>Referto prodotto correttamente.
-Log: registrato errore</t>
   </si>
   <si>
     <t>KO</t>
@@ -416,15 +412,6 @@
     <t>Il campo in esame è sempre presente</t>
   </si>
   <si>
-    <t>2023-04-03T19:17:59Z</t>
-  </si>
-  <si>
-    <t>9125343835b9054b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.30.3e3d996857624ed8372a578fbbc3ac8cdd845e76497e84f7650563bb85698a16.1f532b2541^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Jwt sempre valorizzato con i valori richiesti</t>
   </si>
   <si>
@@ -471,6 +458,12 @@
   </si>
   <si>
     <t>22023-04-04T08:21:07Z</t>
+  </si>
+  <si>
+    <t>L'applicativo è stato aggiornato in modo da salvare in automatico il CF in maiuscolo</t>
+  </si>
+  <si>
+    <t>In caso di timeout (errore 504) l'esecuzione prosegue ed il referto viene prodotto correttamente. Verrà visualizzato sulla richiesta l'esito negativo dell'invio a FSE e l'utente può effettuare il reinvio al momento oppure in un secondo momento</t>
   </si>
 </sst>
 </file>
@@ -1177,35 +1170,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762FDFC5-2362-40DA-8182-D4388668A5DB}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" customWidth="1"/>
-    <col min="4" max="4" width="45.21875" customWidth="1"/>
-    <col min="5" max="5" width="42.77734375" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" customWidth="1"/>
-    <col min="9" max="9" width="29.6640625" customWidth="1"/>
-    <col min="10" max="10" width="19.77734375" customWidth="1"/>
-    <col min="11" max="11" width="34.5546875" customWidth="1"/>
-    <col min="12" max="12" width="25.77734375" customWidth="1"/>
-    <col min="13" max="13" width="31.77734375" customWidth="1"/>
+    <col min="1" max="1" width="4.3046875" customWidth="1"/>
+    <col min="2" max="2" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.53515625" customWidth="1"/>
+    <col min="4" max="4" width="45.23046875" customWidth="1"/>
+    <col min="5" max="5" width="42.765625" customWidth="1"/>
+    <col min="6" max="6" width="21.23046875" customWidth="1"/>
+    <col min="7" max="7" width="15.84375" customWidth="1"/>
+    <col min="8" max="8" width="13.07421875" customWidth="1"/>
+    <col min="9" max="9" width="29.69140625" customWidth="1"/>
+    <col min="10" max="10" width="19.765625" customWidth="1"/>
+    <col min="11" max="11" width="34.53515625" customWidth="1"/>
+    <col min="12" max="12" width="25.765625" customWidth="1"/>
+    <col min="13" max="13" width="31.765625" customWidth="1"/>
     <col min="14" max="14" width="29" customWidth="1"/>
-    <col min="15" max="15" width="29.109375" customWidth="1"/>
-    <col min="16" max="16" width="33.44140625" customWidth="1"/>
-    <col min="17" max="17" width="14.77734375" customWidth="1"/>
+    <col min="15" max="15" width="29.07421875" customWidth="1"/>
+    <col min="16" max="16" width="33.4609375" customWidth="1"/>
+    <col min="17" max="17" width="14.765625" customWidth="1"/>
     <col min="18" max="18" width="26" customWidth="1"/>
-    <col min="19" max="19" width="19.21875" customWidth="1"/>
-    <col min="20" max="20" width="16.109375" customWidth="1"/>
+    <col min="19" max="19" width="19.23046875" customWidth="1"/>
+    <col min="20" max="20" width="16.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.4">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -1227,13 +1220,13 @@
       <c r="S1" s="18"/>
       <c r="T1" s="16"/>
     </row>
-    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="18.45" x14ac:dyDescent="0.4">
       <c r="A2" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="24"/>
       <c r="E2" s="14"/>
@@ -1253,13 +1246,13 @@
       <c r="S2" s="18"/>
       <c r="T2" s="16"/>
     </row>
-    <row r="3" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A3" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="24"/>
       <c r="E3" s="14"/>
@@ -1279,11 +1272,11 @@
       <c r="S3" s="18"/>
       <c r="T3" s="16"/>
     </row>
-    <row r="4" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A4" s="28"/>
       <c r="B4" s="29"/>
       <c r="C4" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="24"/>
       <c r="E4" s="19"/>
@@ -1303,11 +1296,11 @@
       <c r="S4" s="18"/>
       <c r="T4" s="16"/>
     </row>
-    <row r="5" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15.9" x14ac:dyDescent="0.4">
       <c r="A5" s="30"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="24"/>
       <c r="E5" s="14"/>
@@ -1327,7 +1320,7 @@
       <c r="S5" s="18"/>
       <c r="T5" s="16"/>
     </row>
-    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="20"/>
@@ -1349,7 +1342,7 @@
       <c r="S6" s="18"/>
       <c r="T6" s="16"/>
     </row>
-    <row r="7" spans="1:20" ht="37.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="37.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1404,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1431,13 +1424,13 @@
         <v>45020</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>19</v>
@@ -1454,7 +1447,7 @@
         <v>19</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="11"/>
@@ -1463,7 +1456,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1483,13 +1476,13 @@
         <v>45020</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>19</v>
@@ -1506,7 +1499,7 @@
         <v>19</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="R9" s="11"/>
@@ -1515,7 +1508,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1535,13 +1528,13 @@
         <v>45020</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>19</v>
@@ -1558,7 +1551,7 @@
         <v>19</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="11"/>
@@ -1567,7 +1560,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1587,13 +1580,13 @@
         <v>45020</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J11" s="10" t="s">
         <v>19</v>
@@ -1610,7 +1603,7 @@
         <v>19</v>
       </c>
       <c r="P11" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q11" s="10"/>
       <c r="R11" s="11"/>
@@ -1619,7 +1612,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1639,13 +1632,13 @@
         <v>45020</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>19</v>
@@ -1662,7 +1655,7 @@
         <v>19</v>
       </c>
       <c r="P12" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q12" s="10"/>
       <c r="R12" s="11"/>
@@ -1671,7 +1664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>28</v>
       </c>
@@ -1695,7 +1688,7 @@
         <v>29</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
@@ -1706,10 +1699,10 @@
       <c r="R13" s="11"/>
       <c r="S13" s="12"/>
       <c r="T13" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>36</v>
       </c>
@@ -1723,7 +1716,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="9"/>
@@ -1733,7 +1726,7 @@
         <v>29</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -1744,10 +1737,10 @@
       <c r="R14" s="11"/>
       <c r="S14" s="12"/>
       <c r="T14" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>44</v>
       </c>
@@ -1776,16 +1769,16 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="Q15" s="10"/>
       <c r="R15" s="11"/>
       <c r="S15" s="12"/>
       <c r="T15" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>52</v>
       </c>
@@ -1809,7 +1802,7 @@
         <v>29</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -1820,10 +1813,10 @@
       <c r="R16" s="11"/>
       <c r="S16" s="12"/>
       <c r="T16" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>53</v>
       </c>
@@ -1839,43 +1832,29 @@
       <c r="E17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="8">
-        <v>45019</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>82</v>
-      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="10" t="s">
-        <v>29</v>
-      </c>
+      <c r="K17" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>62</v>
-      </c>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="11"/>
       <c r="S17" s="12"/>
       <c r="T17" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>54</v>
       </c>
@@ -1899,7 +1878,7 @@
         <v>29</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
@@ -1910,10 +1889,10 @@
       <c r="R18" s="11"/>
       <c r="S18" s="12"/>
       <c r="T18" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>55</v>
       </c>
@@ -1937,7 +1916,7 @@
         <v>29</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -1948,10 +1927,10 @@
       <c r="R19" s="11"/>
       <c r="S19" s="12"/>
       <c r="T19" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>56</v>
       </c>
@@ -1975,7 +1954,7 @@
         <v>29</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -1986,10 +1965,10 @@
       <c r="R20" s="11"/>
       <c r="S20" s="12"/>
       <c r="T20" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>57</v>
       </c>
@@ -2013,7 +1992,7 @@
         <v>29</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
@@ -2024,10 +2003,10 @@
       <c r="R21" s="11"/>
       <c r="S21" s="12"/>
       <c r="T21" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>58</v>
       </c>
@@ -2051,7 +2030,7 @@
         <v>29</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
@@ -2062,10 +2041,10 @@
       <c r="R22" s="11"/>
       <c r="S22" s="12"/>
       <c r="T22" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>59</v>
       </c>
@@ -2089,7 +2068,7 @@
         <v>29</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
@@ -2100,10 +2079,10 @@
       <c r="R23" s="11"/>
       <c r="S23" s="12"/>
       <c r="T23" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>60</v>
       </c>
@@ -2127,7 +2106,7 @@
         <v>29</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
@@ -2138,10 +2117,10 @@
       <c r="R24" s="11"/>
       <c r="S24" s="12"/>
       <c r="T24" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="67.400000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>61</v>
       </c>
@@ -2165,7 +2144,7 @@
         <v>29</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
@@ -2176,10 +2155,10 @@
       <c r="R25" s="11"/>
       <c r="S25" s="12"/>
       <c r="T25" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" ht="67.349999999999994" customHeight="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="67.400000000000006" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5">
         <v>62</v>
       </c>
@@ -2203,7 +2182,7 @@
         <v>29</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
@@ -2214,7 +2193,7 @@
       <c r="R26" s="11"/>
       <c r="S26" s="12"/>
       <c r="T26" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento gestione casi KO
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
+++ b/GATEWAY/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/report-checklist_WERFEN_MODULAB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://werfen-my.sharepoint.com/personal/mepure_werfen_com/Documents/Documenti/PNRR/NEW_TEST_CASE/A1#111WERFEN00000/WERFEN/MODULAB/4.5.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="197" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8D1B0AD-F5ED-4AF2-9019-9DCBD76A9A03}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="8_{ECEBDF1A-1C3E-4E1F-9A52-8F8D0CCCB9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E6F032B-51DC-4C66-85FD-7F72C97DA563}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15120" xr2:uid="{45719620-2FD1-4552-A135-64BB57A71FCF}"/>
   </bookViews>
@@ -463,7 +463,7 @@
     <t>L'applicativo è stato aggiornato in modo da salvare in automatico il CF in maiuscolo</t>
   </si>
   <si>
-    <t>In caso di timeout (errore 504) l'esecuzione prosegue ed il referto viene prodotto correttamente. Verrà visualizzato sulla richiesta l'esito negativo dell'invio a FSE e l'utente può effettuare il reinvio al momento oppure in un secondo momento</t>
+    <t>In caso di timeout (errore 504) l'esecuzione prosegue ed il referto viene prodotto correttamente. Il re-invio viene eseguito mediante code di gestione che eseguono nuovi tentativi (max 5). Verrà visualizzato sulla richiesta l'esito  dell'invio a FSE e l'utente può effettuare il re-invio in un secondo momento se l'esito negativo non cambia</t>
   </si>
 </sst>
 </file>
@@ -865,10 +865,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1170,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762FDFC5-2362-40DA-8182-D4388668A5DB}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>

</xml_diff>